<commit_message>
mar 16 stonks data
</commit_message>
<xml_diff>
--- a/StonkData.xlsx
+++ b/StonkData.xlsx
@@ -15,6 +15,8 @@
   <sheets>
     <sheet name="Prices from  3 15 2021 1 39 40 " sheetId="5" r:id="rId1"/>
     <sheet name="Prices from  3 15 2021 1 45 11 " sheetId="6" r:id="rId4"/>
+    <sheet name="Prices from  3 16 2021 1 28 01 " sheetId="7" r:id="rId5"/>
+    <sheet name="Prices from  3 16 2021 8 43 57 " sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -3393,4 +3395,2670 @@
   </sheetData>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.377994537353516" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.8009033203125" customWidth="1"/>
+    <col min="5" max="5" width="13.641397476196289" customWidth="1"/>
+    <col min="6" max="6" width="11.8009033203125" customWidth="1"/>
+    <col min="7" max="7" width="11.8009033203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0">
+        <v>25.139999389648438</v>
+      </c>
+      <c r="E2" s="0">
+        <v>25.170000076293945</v>
+      </c>
+      <c r="F2" s="0">
+        <v>25.25</v>
+      </c>
+      <c r="G2" s="0">
+        <v>24.450000762939453</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0">
+        <v>13.510000228881836</v>
+      </c>
+      <c r="E3" s="0">
+        <v>14.039999961853027</v>
+      </c>
+      <c r="F3" s="0">
+        <v>13.609999656677246</v>
+      </c>
+      <c r="G3" s="0">
+        <v>12.34000015258789</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0">
+        <v>83.63999938964844</v>
+      </c>
+      <c r="E4" s="0">
+        <v>82.5</v>
+      </c>
+      <c r="F4" s="0">
+        <v>84.75</v>
+      </c>
+      <c r="G4" s="0">
+        <v>83.11000061035156</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0">
+        <v>22.209999084472656</v>
+      </c>
+      <c r="E5" s="0">
+        <v>22.165000915527344</v>
+      </c>
+      <c r="F5" s="0">
+        <v>22.260000228881836</v>
+      </c>
+      <c r="G5" s="0">
+        <v>20.454999923706055</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0">
+        <v>130.58999633789062</v>
+      </c>
+      <c r="E6" s="0">
+        <v>128.8800048828125</v>
+      </c>
+      <c r="F6" s="0">
+        <v>130.7899932861328</v>
+      </c>
+      <c r="G6" s="0">
+        <v>127.3219985961914</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0">
+        <v>162.52999877929688</v>
+      </c>
+      <c r="E7" s="0">
+        <v>160.74000549316406</v>
+      </c>
+      <c r="F7" s="0">
+        <v>162.82000732421875</v>
+      </c>
+      <c r="G7" s="0">
+        <v>159.42120361328125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0">
+        <v>93.68000030517578</v>
+      </c>
+      <c r="E8" s="0">
+        <v>92.57499694824219</v>
+      </c>
+      <c r="F8" s="0">
+        <v>94.80000305175781</v>
+      </c>
+      <c r="G8" s="0">
+        <v>93.04000091552734</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0">
+        <v>37.52000045776367</v>
+      </c>
+      <c r="E9" s="0">
+        <v>37.75</v>
+      </c>
+      <c r="F9" s="0">
+        <v>37.619998931884766</v>
+      </c>
+      <c r="G9" s="0">
+        <v>36.974998474121094</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.9300000071525574</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.9300000071525574</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.9900000095367432</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.8999999761581421</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0">
+        <v>148.00999450683594</v>
+      </c>
+      <c r="E11" s="0">
+        <v>148.11000061035156</v>
+      </c>
+      <c r="F11" s="0">
+        <v>148.32000732421875</v>
+      </c>
+      <c r="G11" s="0">
+        <v>139.60000610351562</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0">
+        <v>39.83000183105469</v>
+      </c>
+      <c r="E12" s="0">
+        <v>39.84000015258789</v>
+      </c>
+      <c r="F12" s="0">
+        <v>39.900001525878906</v>
+      </c>
+      <c r="G12" s="0">
+        <v>38.88999938964844</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0">
+        <v>51.11000061035156</v>
+      </c>
+      <c r="E13" s="0">
+        <v>50.9900016784668</v>
+      </c>
+      <c r="F13" s="0">
+        <v>51.13999938964844</v>
+      </c>
+      <c r="G13" s="0">
+        <v>49.22999954223633</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0">
+        <v>221.67999267578125</v>
+      </c>
+      <c r="E14" s="0">
+        <v>220.0800018310547</v>
+      </c>
+      <c r="F14" s="0">
+        <v>224.52999877929688</v>
+      </c>
+      <c r="G14" s="0">
+        <v>213.8800048828125</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="0">
+        <v>226.88999938964844</v>
+      </c>
+      <c r="E15" s="0">
+        <v>223.22999572753906</v>
+      </c>
+      <c r="F15" s="0">
+        <v>228</v>
+      </c>
+      <c r="G15" s="0">
+        <v>217.36000061035156</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="0">
+        <v>276</v>
+      </c>
+      <c r="E16" s="0">
+        <v>273.75</v>
+      </c>
+      <c r="F16" s="0">
+        <v>282.1300048828125</v>
+      </c>
+      <c r="G16" s="0">
+        <v>274.9200134277344</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0">
+        <v>267.010009765625</v>
+      </c>
+      <c r="E17" s="0">
+        <v>266.8800048828125</v>
+      </c>
+      <c r="F17" s="0">
+        <v>267.0199890136719</v>
+      </c>
+      <c r="G17" s="0">
+        <v>261.739990234375</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="0">
+        <v>243.72999572753906</v>
+      </c>
+      <c r="E18" s="0">
+        <v>241.30999755859375</v>
+      </c>
+      <c r="F18" s="0">
+        <v>252</v>
+      </c>
+      <c r="G18" s="0">
+        <v>239.01010131835938</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="0">
+        <v>59.150001525878906</v>
+      </c>
+      <c r="E19" s="0">
+        <v>59.02000045776367</v>
+      </c>
+      <c r="F19" s="0">
+        <v>59.4900016784668</v>
+      </c>
+      <c r="G19" s="0">
+        <v>58.849998474121094</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="0">
+        <v>203.27999877929688</v>
+      </c>
+      <c r="E20" s="0">
+        <v>220.13999938964844</v>
+      </c>
+      <c r="F20" s="0">
+        <v>212.99989318847656</v>
+      </c>
+      <c r="G20" s="0">
+        <v>172.35000610351562</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="0">
+        <v>2065.989990234375</v>
+      </c>
+      <c r="E21" s="0">
+        <v>2054.43994140625</v>
+      </c>
+      <c r="F21" s="0">
+        <v>2112.989990234375</v>
+      </c>
+      <c r="G21" s="0">
+        <v>2059.2900390625</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="0">
+        <v>89.19999694824219</v>
+      </c>
+      <c r="E22" s="0">
+        <v>89.05999755859375</v>
+      </c>
+      <c r="F22" s="0">
+        <v>89.19999694824219</v>
+      </c>
+      <c r="G22" s="0">
+        <v>86.31999969482422</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0">
+        <v>278.8900146484375</v>
+      </c>
+      <c r="E23" s="0">
+        <v>278.5400085449219</v>
+      </c>
+      <c r="F23" s="0">
+        <v>282.2300109863281</v>
+      </c>
+      <c r="G23" s="0">
+        <v>277.6499938964844</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="0">
+        <v>51.20000076293945</v>
+      </c>
+      <c r="E24" s="0">
+        <v>51.029998779296875</v>
+      </c>
+      <c r="F24" s="0">
+        <v>51.474998474121094</v>
+      </c>
+      <c r="G24" s="0">
+        <v>51.040000915527344</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="0">
+        <v>110.8499984741211</v>
+      </c>
+      <c r="E25" s="0">
+        <v>109.9800033569336</v>
+      </c>
+      <c r="F25" s="0">
+        <v>113.16000366210938</v>
+      </c>
+      <c r="G25" s="0">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="0">
+        <v>62.13999938964844</v>
+      </c>
+      <c r="E26" s="0">
+        <v>62.099998474121094</v>
+      </c>
+      <c r="F26" s="0">
+        <v>62.29999923706055</v>
+      </c>
+      <c r="G26" s="0">
+        <v>60.59000015258789</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="0">
+        <v>219.57000732421875</v>
+      </c>
+      <c r="E27" s="0">
+        <v>220.4600067138672</v>
+      </c>
+      <c r="F27" s="0">
+        <v>221.29800415039062</v>
+      </c>
+      <c r="G27" s="0">
+        <v>217.16000366210938</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="0">
+        <v>148.5</v>
+      </c>
+      <c r="E28" s="0">
+        <v>143.66000366210938</v>
+      </c>
+      <c r="F28" s="0">
+        <v>157.74000549316406</v>
+      </c>
+      <c r="G28" s="0">
+        <v>145.875</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="0">
+        <v>236.3800048828125</v>
+      </c>
+      <c r="E29" s="0">
+        <v>234.80999755859375</v>
+      </c>
+      <c r="F29" s="0">
+        <v>240.0500030517578</v>
+      </c>
+      <c r="G29" s="0">
+        <v>235.94000244140625</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="0">
+        <v>220</v>
+      </c>
+      <c r="E30" s="0">
+        <v>217.4600067138672</v>
+      </c>
+      <c r="F30" s="0">
+        <v>235</v>
+      </c>
+      <c r="G30" s="0">
+        <v>218.5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="0">
+        <v>535.530029296875</v>
+      </c>
+      <c r="E31" s="0">
+        <v>527.6500244140625</v>
+      </c>
+      <c r="F31" s="0">
+        <v>540.489990234375</v>
+      </c>
+      <c r="G31" s="0">
+        <v>530.3200073242188</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="0">
+        <v>28.649999618530273</v>
+      </c>
+      <c r="E32" s="0">
+        <v>28.809999465942383</v>
+      </c>
+      <c r="F32" s="0">
+        <v>30.039899826049805</v>
+      </c>
+      <c r="G32" s="0">
+        <v>28.6200008392334</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="0">
+        <v>35.470001220703125</v>
+      </c>
+      <c r="E33" s="0">
+        <v>35.40999984741211</v>
+      </c>
+      <c r="F33" s="0">
+        <v>35.83000183105469</v>
+      </c>
+      <c r="G33" s="0">
+        <v>35.310001373291016</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="0">
+        <v>73.98999786376953</v>
+      </c>
+      <c r="E34" s="0">
+        <v>72.79000091552734</v>
+      </c>
+      <c r="F34" s="0">
+        <v>75.09829711914062</v>
+      </c>
+      <c r="G34" s="0">
+        <v>72.87999725341797</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="0">
+        <v>18.950000762939453</v>
+      </c>
+      <c r="E35" s="0">
+        <v>18.709999084472656</v>
+      </c>
+      <c r="F35" s="0">
+        <v>18.969999313354492</v>
+      </c>
+      <c r="G35" s="0">
+        <v>17.700000762939453</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="0">
+        <v>321.2300109863281</v>
+      </c>
+      <c r="E36" s="0">
+        <v>318.8299865722656</v>
+      </c>
+      <c r="F36" s="0">
+        <v>324.20001220703125</v>
+      </c>
+      <c r="G36" s="0">
+        <v>320.44000244140625</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="0">
+        <v>75.43000030517578</v>
+      </c>
+      <c r="E37" s="0">
+        <v>74.86000061035156</v>
+      </c>
+      <c r="F37" s="0">
+        <v>76.80000305175781</v>
+      </c>
+      <c r="G37" s="0">
+        <v>74.30999755859375</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="0">
+        <v>110.68000030517578</v>
+      </c>
+      <c r="E38" s="0">
+        <v>108.9000015258789</v>
+      </c>
+      <c r="F38" s="0">
+        <v>112.33999633789062</v>
+      </c>
+      <c r="G38" s="0">
+        <v>109.88999938964844</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="0">
+        <v>1182</v>
+      </c>
+      <c r="E39" s="0">
+        <v>1159</v>
+      </c>
+      <c r="F39" s="0">
+        <v>1190</v>
+      </c>
+      <c r="G39" s="0">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="0">
+        <v>148.4499969482422</v>
+      </c>
+      <c r="E40" s="0">
+        <v>146.97000122070312</v>
+      </c>
+      <c r="F40" s="0">
+        <v>149.97999572753906</v>
+      </c>
+      <c r="G40" s="0">
+        <v>137.55630493164062</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="0">
+        <v>1.7400000095367432</v>
+      </c>
+      <c r="E41" s="0">
+        <v>1.6200000047683716</v>
+      </c>
+      <c r="F41" s="0">
+        <v>1.75</v>
+      </c>
+      <c r="G41" s="0">
+        <v>1.5499999523162842</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="0">
+        <v>252.25999450683594</v>
+      </c>
+      <c r="E42" s="0">
+        <v>251.22999572753906</v>
+      </c>
+      <c r="F42" s="0">
+        <v>252.5</v>
+      </c>
+      <c r="G42" s="0">
+        <v>244.17999267578125</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="0">
+        <v>48.86000061035156</v>
+      </c>
+      <c r="E43" s="0">
+        <v>48.54999923706055</v>
+      </c>
+      <c r="F43" s="0">
+        <v>48.8650016784668</v>
+      </c>
+      <c r="G43" s="0">
+        <v>47.08000183105469</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="0">
+        <v>82.22000122070312</v>
+      </c>
+      <c r="E44" s="0">
+        <v>83.23999786376953</v>
+      </c>
+      <c r="F44" s="0">
+        <v>82.63999938964844</v>
+      </c>
+      <c r="G44" s="0">
+        <v>80.4000015258789</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="0">
+        <v>112.87000274658203</v>
+      </c>
+      <c r="E45" s="0">
+        <v>109.66999816894531</v>
+      </c>
+      <c r="F45" s="0">
+        <v>114.11000061035156</v>
+      </c>
+      <c r="G45" s="0">
+        <v>110.12999725341797</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="0">
+        <v>36.400001525878906</v>
+      </c>
+      <c r="E46" s="0">
+        <v>36.779998779296875</v>
+      </c>
+      <c r="F46" s="0">
+        <v>37.61989974975586</v>
+      </c>
+      <c r="G46" s="0">
+        <v>35.38999938964844</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="0">
+        <v>162.94500732421875</v>
+      </c>
+      <c r="E47" s="0">
+        <v>162.63999938964844</v>
+      </c>
+      <c r="F47" s="0">
+        <v>163.8800048828125</v>
+      </c>
+      <c r="G47" s="0">
+        <v>161.42999267578125</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="0">
+        <v>1.7400000095367432</v>
+      </c>
+      <c r="E48" s="0">
+        <v>1.7300000190734863</v>
+      </c>
+      <c r="F48" s="0">
+        <v>1.75</v>
+      </c>
+      <c r="G48" s="0">
+        <v>1.667099952697754</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="0">
+        <v>56.209999084472656</v>
+      </c>
+      <c r="E49" s="0">
+        <v>56.650001525878906</v>
+      </c>
+      <c r="F49" s="0">
+        <v>56.650001525878906</v>
+      </c>
+      <c r="G49" s="0">
+        <v>53.93000030517578</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="0">
+        <v>39.33000183105469</v>
+      </c>
+      <c r="E50" s="0">
+        <v>39.70000076293945</v>
+      </c>
+      <c r="F50" s="0">
+        <v>39.38999938964844</v>
+      </c>
+      <c r="G50" s="0">
+        <v>38.720001220703125</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="0">
+        <v>129.60000610351562</v>
+      </c>
+      <c r="E51" s="0">
+        <v>128.4199981689453</v>
+      </c>
+      <c r="F51" s="0">
+        <v>130.97000122070312</v>
+      </c>
+      <c r="G51" s="0">
+        <v>127.51000213623047</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="0">
+        <v>122.72000122070312</v>
+      </c>
+      <c r="E52" s="0">
+        <v>122.62000274658203</v>
+      </c>
+      <c r="F52" s="0">
+        <v>123.13990020751953</v>
+      </c>
+      <c r="G52" s="0">
+        <v>122.2300033569336</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="0">
+        <v>132.82000732421875</v>
+      </c>
+      <c r="E53" s="0">
+        <v>133.42999267578125</v>
+      </c>
+      <c r="F53" s="0">
+        <v>134.27999877929688</v>
+      </c>
+      <c r="G53" s="0">
+        <v>132.82000732421875</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="0">
+        <v>23</v>
+      </c>
+      <c r="E54" s="0">
+        <v>23.139999389648438</v>
+      </c>
+      <c r="F54" s="0">
+        <v>23.079999923706055</v>
+      </c>
+      <c r="G54" s="0">
+        <v>21.520000457763672</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="0">
+        <v>148.9600067138672</v>
+      </c>
+      <c r="E55" s="0">
+        <v>148.22000122070312</v>
+      </c>
+      <c r="F55" s="0">
+        <v>149.23500061035156</v>
+      </c>
+      <c r="G55" s="0">
+        <v>146.77999877929688</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="0">
+        <v>153.24000549316406</v>
+      </c>
+      <c r="E56" s="0">
+        <v>150.5</v>
+      </c>
+      <c r="F56" s="0">
+        <v>156.83999633789062</v>
+      </c>
+      <c r="G56" s="0">
+        <v>146.4550018310547</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="0">
+        <v>159.8800048828125</v>
+      </c>
+      <c r="E57" s="0">
+        <v>155.99000549316406</v>
+      </c>
+      <c r="F57" s="0">
+        <v>162</v>
+      </c>
+      <c r="G57" s="0">
+        <v>151.72000122070312</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.377994537353516" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.8009033203125" customWidth="1"/>
+    <col min="5" max="5" width="13.641397476196289" customWidth="1"/>
+    <col min="6" max="6" width="11.8009033203125" customWidth="1"/>
+    <col min="7" max="7" width="11.8009033203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0">
+        <v>25.110000610351562</v>
+      </c>
+      <c r="E2" s="0">
+        <v>25.170000076293945</v>
+      </c>
+      <c r="F2" s="0">
+        <v>25.25</v>
+      </c>
+      <c r="G2" s="0">
+        <v>24.309999465942383</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0">
+        <v>13.619999885559082</v>
+      </c>
+      <c r="E3" s="0">
+        <v>14.039999961853027</v>
+      </c>
+      <c r="F3" s="0">
+        <v>13.619999885559082</v>
+      </c>
+      <c r="G3" s="0">
+        <v>12.34000015258789</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0">
+        <v>83.66000366210938</v>
+      </c>
+      <c r="E4" s="0">
+        <v>82.5</v>
+      </c>
+      <c r="F4" s="0">
+        <v>84.75</v>
+      </c>
+      <c r="G4" s="0">
+        <v>82.25499725341797</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0">
+        <v>22.25</v>
+      </c>
+      <c r="E5" s="0">
+        <v>22.165000915527344</v>
+      </c>
+      <c r="F5" s="0">
+        <v>22.260000228881836</v>
+      </c>
+      <c r="G5" s="0">
+        <v>19.940000534057617</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0">
+        <v>130.50999450683594</v>
+      </c>
+      <c r="E6" s="0">
+        <v>128.8800048828125</v>
+      </c>
+      <c r="F6" s="0">
+        <v>130.8000030517578</v>
+      </c>
+      <c r="G6" s="0">
+        <v>123.9800033569336</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0">
+        <v>162.47999572753906</v>
+      </c>
+      <c r="E7" s="0">
+        <v>160.74000549316406</v>
+      </c>
+      <c r="F7" s="0">
+        <v>162.89999389648438</v>
+      </c>
+      <c r="G7" s="0">
+        <v>155.8000030517578</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0">
+        <v>93.55999755859375</v>
+      </c>
+      <c r="E8" s="0">
+        <v>92.57499694824219</v>
+      </c>
+      <c r="F8" s="0">
+        <v>94.80000305175781</v>
+      </c>
+      <c r="G8" s="0">
+        <v>92.92500305175781</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0">
+        <v>37.41999816894531</v>
+      </c>
+      <c r="E9" s="0">
+        <v>37.75</v>
+      </c>
+      <c r="F9" s="0">
+        <v>37.720001220703125</v>
+      </c>
+      <c r="G9" s="0">
+        <v>36.970001220703125</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.9300000071525574</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.9300000071525574</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.9900000095367432</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.8809999823570251</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0">
+        <v>148.00999450683594</v>
+      </c>
+      <c r="E11" s="0">
+        <v>148.11000061035156</v>
+      </c>
+      <c r="F11" s="0">
+        <v>148.32000732421875</v>
+      </c>
+      <c r="G11" s="0">
+        <v>137.00999450683594</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0">
+        <v>39.83000183105469</v>
+      </c>
+      <c r="E12" s="0">
+        <v>39.84000015258789</v>
+      </c>
+      <c r="F12" s="0">
+        <v>40.22999954223633</v>
+      </c>
+      <c r="G12" s="0">
+        <v>38.88999938964844</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0">
+        <v>51.040000915527344</v>
+      </c>
+      <c r="E13" s="0">
+        <v>50.9900016784668</v>
+      </c>
+      <c r="F13" s="0">
+        <v>51.13999938964844</v>
+      </c>
+      <c r="G13" s="0">
+        <v>49.029998779296875</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0">
+        <v>221.67999267578125</v>
+      </c>
+      <c r="E14" s="0">
+        <v>220.0800018310547</v>
+      </c>
+      <c r="F14" s="0">
+        <v>224.52999877929688</v>
+      </c>
+      <c r="G14" s="0">
+        <v>210.16000366210938</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="0">
+        <v>226.88999938964844</v>
+      </c>
+      <c r="E15" s="0">
+        <v>223.22999572753906</v>
+      </c>
+      <c r="F15" s="0">
+        <v>228</v>
+      </c>
+      <c r="G15" s="0">
+        <v>210.75</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="0">
+        <v>276.0849914550781</v>
+      </c>
+      <c r="E16" s="0">
+        <v>273.75</v>
+      </c>
+      <c r="F16" s="0">
+        <v>282.1400146484375</v>
+      </c>
+      <c r="G16" s="0">
+        <v>274.79998779296875</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0">
+        <v>267</v>
+      </c>
+      <c r="E17" s="0">
+        <v>266.8800048828125</v>
+      </c>
+      <c r="F17" s="0">
+        <v>267.0299987792969</v>
+      </c>
+      <c r="G17" s="0">
+        <v>260.29998779296875</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="0">
+        <v>243.0399932861328</v>
+      </c>
+      <c r="E18" s="0">
+        <v>241.30999755859375</v>
+      </c>
+      <c r="F18" s="0">
+        <v>252</v>
+      </c>
+      <c r="G18" s="0">
+        <v>229.02000427246094</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="0">
+        <v>59</v>
+      </c>
+      <c r="E19" s="0">
+        <v>59.02000045776367</v>
+      </c>
+      <c r="F19" s="0">
+        <v>59.720001220703125</v>
+      </c>
+      <c r="G19" s="0">
+        <v>58.849998474121094</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="0">
+        <v>203.16000366210938</v>
+      </c>
+      <c r="E20" s="0">
+        <v>220.13999938964844</v>
+      </c>
+      <c r="F20" s="0">
+        <v>220.6999969482422</v>
+      </c>
+      <c r="G20" s="0">
+        <v>172.35000610351562</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="0">
+        <v>2065.989990234375</v>
+      </c>
+      <c r="E21" s="0">
+        <v>2054.43994140625</v>
+      </c>
+      <c r="F21" s="0">
+        <v>2113.679931640625</v>
+      </c>
+      <c r="G21" s="0">
+        <v>2059.2900390625</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="0">
+        <v>89.25</v>
+      </c>
+      <c r="E22" s="0">
+        <v>89.05999755859375</v>
+      </c>
+      <c r="F22" s="0">
+        <v>89.25</v>
+      </c>
+      <c r="G22" s="0">
+        <v>85.87999725341797</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0">
+        <v>278.5400085449219</v>
+      </c>
+      <c r="E23" s="0">
+        <v>278.5400085449219</v>
+      </c>
+      <c r="F23" s="0">
+        <v>282.5199890136719</v>
+      </c>
+      <c r="G23" s="0">
+        <v>277.6499938964844</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="0">
+        <v>51.20000076293945</v>
+      </c>
+      <c r="E24" s="0">
+        <v>51.029998779296875</v>
+      </c>
+      <c r="F24" s="0">
+        <v>51.52000045776367</v>
+      </c>
+      <c r="G24" s="0">
+        <v>51.040000915527344</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="0">
+        <v>110</v>
+      </c>
+      <c r="E25" s="0">
+        <v>109.9800033569336</v>
+      </c>
+      <c r="F25" s="0">
+        <v>113.16999816894531</v>
+      </c>
+      <c r="G25" s="0">
+        <v>105.05999755859375</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="0">
+        <v>62.2599983215332</v>
+      </c>
+      <c r="E26" s="0">
+        <v>62.099998474121094</v>
+      </c>
+      <c r="F26" s="0">
+        <v>62.29999923706055</v>
+      </c>
+      <c r="G26" s="0">
+        <v>60.529998779296875</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="0">
+        <v>219.5800018310547</v>
+      </c>
+      <c r="E27" s="0">
+        <v>220.4600067138672</v>
+      </c>
+      <c r="F27" s="0">
+        <v>221.3000030517578</v>
+      </c>
+      <c r="G27" s="0">
+        <v>217.16000366210938</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="0">
+        <v>148.5</v>
+      </c>
+      <c r="E28" s="0">
+        <v>143.66000366210938</v>
+      </c>
+      <c r="F28" s="0">
+        <v>157.75</v>
+      </c>
+      <c r="G28" s="0">
+        <v>145.83999633789062</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="0">
+        <v>236.27999877929688</v>
+      </c>
+      <c r="E29" s="0">
+        <v>234.80999755859375</v>
+      </c>
+      <c r="F29" s="0">
+        <v>240.05499267578125</v>
+      </c>
+      <c r="G29" s="0">
+        <v>235.94000244140625</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="0">
+        <v>220.05999755859375</v>
+      </c>
+      <c r="E30" s="0">
+        <v>217.4600067138672</v>
+      </c>
+      <c r="F30" s="0">
+        <v>235</v>
+      </c>
+      <c r="G30" s="0">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="0">
+        <v>534.260009765625</v>
+      </c>
+      <c r="E31" s="0">
+        <v>527.6500244140625</v>
+      </c>
+      <c r="F31" s="0">
+        <v>540.5</v>
+      </c>
+      <c r="G31" s="0">
+        <v>524.6699829101562</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="0">
+        <v>28.649999618530273</v>
+      </c>
+      <c r="E32" s="0">
+        <v>28.809999465942383</v>
+      </c>
+      <c r="F32" s="0">
+        <v>30.040000915527344</v>
+      </c>
+      <c r="G32" s="0">
+        <v>26.440000534057617</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="0">
+        <v>35.470001220703125</v>
+      </c>
+      <c r="E33" s="0">
+        <v>35.40999984741211</v>
+      </c>
+      <c r="F33" s="0">
+        <v>35.86000061035156</v>
+      </c>
+      <c r="G33" s="0">
+        <v>35.310001373291016</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="0">
+        <v>73.98999786376953</v>
+      </c>
+      <c r="E34" s="0">
+        <v>72.79000091552734</v>
+      </c>
+      <c r="F34" s="0">
+        <v>75.09829711914062</v>
+      </c>
+      <c r="G34" s="0">
+        <v>72.51000213623047</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="0">
+        <v>18.950000762939453</v>
+      </c>
+      <c r="E35" s="0">
+        <v>18.709999084472656</v>
+      </c>
+      <c r="F35" s="0">
+        <v>18.969999313354492</v>
+      </c>
+      <c r="G35" s="0">
+        <v>17.329999923706055</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="0">
+        <v>321.0899963378906</v>
+      </c>
+      <c r="E36" s="0">
+        <v>318.8299865722656</v>
+      </c>
+      <c r="F36" s="0">
+        <v>324.20001220703125</v>
+      </c>
+      <c r="G36" s="0">
+        <v>319.1000061035156</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="0">
+        <v>75.43000030517578</v>
+      </c>
+      <c r="E37" s="0">
+        <v>74.86000061035156</v>
+      </c>
+      <c r="F37" s="0">
+        <v>76.80000305175781</v>
+      </c>
+      <c r="G37" s="0">
+        <v>71.87999725341797</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="0">
+        <v>110.56800079345703</v>
+      </c>
+      <c r="E38" s="0">
+        <v>108.9000015258789</v>
+      </c>
+      <c r="F38" s="0">
+        <v>112.33999633789062</v>
+      </c>
+      <c r="G38" s="0">
+        <v>109.88999938964844</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="0">
+        <v>1183.1199951171875</v>
+      </c>
+      <c r="E39" s="0">
+        <v>1159</v>
+      </c>
+      <c r="F39" s="0">
+        <v>1190</v>
+      </c>
+      <c r="G39" s="0">
+        <v>1124.0001220703125</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="0">
+        <v>148.5</v>
+      </c>
+      <c r="E40" s="0">
+        <v>146.97000122070312</v>
+      </c>
+      <c r="F40" s="0">
+        <v>149.97999572753906</v>
+      </c>
+      <c r="G40" s="0">
+        <v>137.55630493164062</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="0">
+        <v>1.7450000047683716</v>
+      </c>
+      <c r="E41" s="0">
+        <v>1.6200000047683716</v>
+      </c>
+      <c r="F41" s="0">
+        <v>1.75</v>
+      </c>
+      <c r="G41" s="0">
+        <v>1.4500000476837158</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="0">
+        <v>252.25999450683594</v>
+      </c>
+      <c r="E42" s="0">
+        <v>251.22999572753906</v>
+      </c>
+      <c r="F42" s="0">
+        <v>252.5</v>
+      </c>
+      <c r="G42" s="0">
+        <v>238.6699981689453</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="0">
+        <v>48.86000061035156</v>
+      </c>
+      <c r="E43" s="0">
+        <v>48.54999923706055</v>
+      </c>
+      <c r="F43" s="0">
+        <v>48.8650016784668</v>
+      </c>
+      <c r="G43" s="0">
+        <v>46.81999969482422</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="0">
+        <v>82.37999725341797</v>
+      </c>
+      <c r="E44" s="0">
+        <v>83.23999786376953</v>
+      </c>
+      <c r="F44" s="0">
+        <v>82.63999938964844</v>
+      </c>
+      <c r="G44" s="0">
+        <v>80.16999816894531</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="0">
+        <v>112.87999725341797</v>
+      </c>
+      <c r="E45" s="0">
+        <v>109.66999816894531</v>
+      </c>
+      <c r="F45" s="0">
+        <v>114.13999938964844</v>
+      </c>
+      <c r="G45" s="0">
+        <v>106.66999816894531</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="0">
+        <v>36.400001525878906</v>
+      </c>
+      <c r="E46" s="0">
+        <v>36.779998779296875</v>
+      </c>
+      <c r="F46" s="0">
+        <v>37.64860153198242</v>
+      </c>
+      <c r="G46" s="0">
+        <v>34.82339859008789</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="0">
+        <v>162.77999877929688</v>
+      </c>
+      <c r="E47" s="0">
+        <v>162.63999938964844</v>
+      </c>
+      <c r="F47" s="0">
+        <v>164.16000366210938</v>
+      </c>
+      <c r="G47" s="0">
+        <v>161.42999267578125</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="0">
+        <v>1.7400000095367432</v>
+      </c>
+      <c r="E48" s="0">
+        <v>1.7300000190734863</v>
+      </c>
+      <c r="F48" s="0">
+        <v>1.75</v>
+      </c>
+      <c r="G48" s="0">
+        <v>1.667099952697754</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="0">
+        <v>56.209999084472656</v>
+      </c>
+      <c r="E49" s="0">
+        <v>56.650001525878906</v>
+      </c>
+      <c r="F49" s="0">
+        <v>56.709999084472656</v>
+      </c>
+      <c r="G49" s="0">
+        <v>52.83000183105469</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="0">
+        <v>39.369998931884766</v>
+      </c>
+      <c r="E50" s="0">
+        <v>39.70000076293945</v>
+      </c>
+      <c r="F50" s="0">
+        <v>39.4900016784668</v>
+      </c>
+      <c r="G50" s="0">
+        <v>38.720001220703125</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="0">
+        <v>129.60000610351562</v>
+      </c>
+      <c r="E51" s="0">
+        <v>128.4199981689453</v>
+      </c>
+      <c r="F51" s="0">
+        <v>131.3000030517578</v>
+      </c>
+      <c r="G51" s="0">
+        <v>127.51000213623047</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="0">
+        <v>122.70999908447266</v>
+      </c>
+      <c r="E52" s="0">
+        <v>122.62000274658203</v>
+      </c>
+      <c r="F52" s="0">
+        <v>123.13990020751953</v>
+      </c>
+      <c r="G52" s="0">
+        <v>122.19999694824219</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="0">
+        <v>132.82000732421875</v>
+      </c>
+      <c r="E53" s="0">
+        <v>133.42999267578125</v>
+      </c>
+      <c r="F53" s="0">
+        <v>134.27999877929688</v>
+      </c>
+      <c r="G53" s="0">
+        <v>132.82000732421875</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="0">
+        <v>22.979999542236328</v>
+      </c>
+      <c r="E54" s="0">
+        <v>23.139999389648438</v>
+      </c>
+      <c r="F54" s="0">
+        <v>23.079999923706055</v>
+      </c>
+      <c r="G54" s="0">
+        <v>21.100000381469727</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="0">
+        <v>148.75999450683594</v>
+      </c>
+      <c r="E55" s="0">
+        <v>148.22000122070312</v>
+      </c>
+      <c r="F55" s="0">
+        <v>149.23500061035156</v>
+      </c>
+      <c r="G55" s="0">
+        <v>143.22999572753906</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="0">
+        <v>153.24000549316406</v>
+      </c>
+      <c r="E56" s="0">
+        <v>150.5</v>
+      </c>
+      <c r="F56" s="0">
+        <v>156.83999633789062</v>
+      </c>
+      <c r="G56" s="0">
+        <v>142.125</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="0">
+        <v>159.8800048828125</v>
+      </c>
+      <c r="E57" s="0">
+        <v>155.99000549316406</v>
+      </c>
+      <c r="F57" s="0">
+        <v>162</v>
+      </c>
+      <c r="G57" s="0">
+        <v>147.08999633789062</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
another day another dollar lost
</commit_message>
<xml_diff>
--- a/StonkData.xlsx
+++ b/StonkData.xlsx
@@ -21,6 +21,8 @@
     <sheet name="Prices from  3 19 2021 8 04 47 " sheetId="10" r:id="rId8"/>
     <sheet name="Prices from  3 23 2021 1 01 01 " sheetId="11" r:id="rId9"/>
     <sheet name="Prices from  3 23 2021 8 10 25 " sheetId="12" r:id="rId10"/>
+    <sheet name="Prices from  3 25 2021 8 08 52 " sheetId="13" r:id="rId11"/>
+    <sheet name="Prices from  3 25 2021 9 32 39 " sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -6067,6 +6069,2672 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.377994537353516" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.8009033203125" customWidth="1"/>
+    <col min="5" max="5" width="13.641397476196289" customWidth="1"/>
+    <col min="6" max="6" width="10.707245826721191" customWidth="1"/>
+    <col min="7" max="7" width="11.8009033203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0">
+        <v>22.790000915527344</v>
+      </c>
+      <c r="E2" s="0">
+        <v>22.270000457763672</v>
+      </c>
+      <c r="F2" s="0">
+        <v>23.18000030517578</v>
+      </c>
+      <c r="G2" s="0">
+        <v>21.760000228881836</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0">
+        <v>10.819999694824219</v>
+      </c>
+      <c r="E3" s="0">
+        <v>10.65999984741211</v>
+      </c>
+      <c r="F3" s="0">
+        <v>11.210000038146973</v>
+      </c>
+      <c r="G3" s="0">
+        <v>8.930000305175781</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0">
+        <v>77.55000305175781</v>
+      </c>
+      <c r="E4" s="0">
+        <v>78.37999725341797</v>
+      </c>
+      <c r="F4" s="0">
+        <v>78.80000305175781</v>
+      </c>
+      <c r="G4" s="0">
+        <v>76.4000015258789</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0">
+        <v>18.260000228881836</v>
+      </c>
+      <c r="E5" s="0">
+        <v>18.1200008392334</v>
+      </c>
+      <c r="F5" s="0">
+        <v>18.6200008392334</v>
+      </c>
+      <c r="G5" s="0">
+        <v>17.3700008392334</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0">
+        <v>122.5</v>
+      </c>
+      <c r="E6" s="0">
+        <v>121.69999694824219</v>
+      </c>
+      <c r="F6" s="0">
+        <v>122.68000030517578</v>
+      </c>
+      <c r="G6" s="0">
+        <v>114.55000305175781</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0">
+        <v>152.5500030517578</v>
+      </c>
+      <c r="E7" s="0">
+        <v>151.25999450683594</v>
+      </c>
+      <c r="F7" s="0">
+        <v>152.5500030517578</v>
+      </c>
+      <c r="G7" s="0">
+        <v>142.25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0">
+        <v>91.55000305175781</v>
+      </c>
+      <c r="E8" s="0">
+        <v>91.37999725341797</v>
+      </c>
+      <c r="F8" s="0">
+        <v>91.55000305175781</v>
+      </c>
+      <c r="G8" s="0">
+        <v>89.66999816894531</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0">
+        <v>37.209999084472656</v>
+      </c>
+      <c r="E9" s="0">
+        <v>36.900001525878906</v>
+      </c>
+      <c r="F9" s="0">
+        <v>37.790000915527344</v>
+      </c>
+      <c r="G9" s="0">
+        <v>36.88999938964844</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.8403000235557556</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.8700000047683716</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.9100000262260437</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.8299999833106995</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0">
+        <v>136</v>
+      </c>
+      <c r="E11" s="0">
+        <v>137.10000610351562</v>
+      </c>
+      <c r="F11" s="0">
+        <v>136.77000427246094</v>
+      </c>
+      <c r="G11" s="0">
+        <v>129.64810180664062</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0">
+        <v>37.959999084472656</v>
+      </c>
+      <c r="E12" s="0">
+        <v>37.68000030517578</v>
+      </c>
+      <c r="F12" s="0">
+        <v>38.79999923706055</v>
+      </c>
+      <c r="G12" s="0">
+        <v>36.970001220703125</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0">
+        <v>46.540000915527344</v>
+      </c>
+      <c r="E13" s="0">
+        <v>45.63999938964844</v>
+      </c>
+      <c r="F13" s="0">
+        <v>47.399898529052734</v>
+      </c>
+      <c r="G13" s="0">
+        <v>45.560001373291016</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0">
+        <v>209</v>
+      </c>
+      <c r="E14" s="0">
+        <v>207.9600067138672</v>
+      </c>
+      <c r="F14" s="0">
+        <v>209</v>
+      </c>
+      <c r="G14" s="0">
+        <v>198.02000427246094</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="0">
+        <v>220.85000610351562</v>
+      </c>
+      <c r="E15" s="0">
+        <v>219.6699981689453</v>
+      </c>
+      <c r="F15" s="0">
+        <v>221</v>
+      </c>
+      <c r="G15" s="0">
+        <v>197.8699951171875</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="0">
+        <v>291</v>
+      </c>
+      <c r="E16" s="0">
+        <v>290.6300048828125</v>
+      </c>
+      <c r="F16" s="0">
+        <v>291.7200012207031</v>
+      </c>
+      <c r="G16" s="0">
+        <v>281.1600036621094</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0">
+        <v>269</v>
+      </c>
+      <c r="E17" s="0">
+        <v>266.80999755859375</v>
+      </c>
+      <c r="F17" s="0">
+        <v>274.27398681640625</v>
+      </c>
+      <c r="G17" s="0">
+        <v>267.3999938964844</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="0">
+        <v>223.41000366210938</v>
+      </c>
+      <c r="E18" s="0">
+        <v>220.77999877929688</v>
+      </c>
+      <c r="F18" s="0">
+        <v>223.41000366210938</v>
+      </c>
+      <c r="G18" s="0">
+        <v>201.8800048828125</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="0">
+        <v>58.52000045776367</v>
+      </c>
+      <c r="E19" s="0">
+        <v>61.189998626708984</v>
+      </c>
+      <c r="F19" s="0">
+        <v>59.47999954223633</v>
+      </c>
+      <c r="G19" s="0">
+        <v>57.810001373291016</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="0">
+        <v>157.97999572753906</v>
+      </c>
+      <c r="E20" s="0">
+        <v>181.75</v>
+      </c>
+      <c r="F20" s="0">
+        <v>166.97000122070312</v>
+      </c>
+      <c r="G20" s="0">
+        <v>118.62000274658203</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="0">
+        <v>2051.760009765625</v>
+      </c>
+      <c r="E21" s="0">
+        <v>2041.3299560546875</v>
+      </c>
+      <c r="F21" s="0">
+        <v>2067.60009765625</v>
+      </c>
+      <c r="G21" s="0">
+        <v>2029.0001220703125</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="0">
+        <v>81.05999755859375</v>
+      </c>
+      <c r="E22" s="0">
+        <v>79.80999755859375</v>
+      </c>
+      <c r="F22" s="0">
+        <v>82.7699966430664</v>
+      </c>
+      <c r="G22" s="0">
+        <v>80.0999984741211</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0">
+        <v>289.260009765625</v>
+      </c>
+      <c r="E23" s="0">
+        <v>289.9800109863281</v>
+      </c>
+      <c r="F23" s="0">
+        <v>296.77899169921875</v>
+      </c>
+      <c r="G23" s="0">
+        <v>288.989990234375</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="0">
+        <v>51.16999816894531</v>
+      </c>
+      <c r="E24" s="0">
+        <v>51.38999938964844</v>
+      </c>
+      <c r="F24" s="0">
+        <v>51.88999938964844</v>
+      </c>
+      <c r="G24" s="0">
+        <v>51.150001525878906</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="0">
+        <v>96.30999755859375</v>
+      </c>
+      <c r="E25" s="0">
+        <v>95.87999725341797</v>
+      </c>
+      <c r="F25" s="0">
+        <v>97.79000091552734</v>
+      </c>
+      <c r="G25" s="0">
+        <v>88.11000061035156</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="0">
+        <v>58.59000015258789</v>
+      </c>
+      <c r="E26" s="0">
+        <v>57.619998931884766</v>
+      </c>
+      <c r="F26" s="0">
+        <v>59.65999984741211</v>
+      </c>
+      <c r="G26" s="0">
+        <v>57.689998626708984</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="0">
+        <v>225.32000732421875</v>
+      </c>
+      <c r="E27" s="0">
+        <v>224.3699951171875</v>
+      </c>
+      <c r="F27" s="0">
+        <v>227.02000427246094</v>
+      </c>
+      <c r="G27" s="0">
+        <v>224.0399932861328</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="0">
+        <v>137.25</v>
+      </c>
+      <c r="E28" s="0">
+        <v>136.52000427246094</v>
+      </c>
+      <c r="F28" s="0">
+        <v>137.74000549316406</v>
+      </c>
+      <c r="G28" s="0">
+        <v>131.00999450683594</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="0">
+        <v>237.84500122070312</v>
+      </c>
+      <c r="E29" s="0">
+        <v>237.5800018310547</v>
+      </c>
+      <c r="F29" s="0">
+        <v>238</v>
+      </c>
+      <c r="G29" s="0">
+        <v>235.32000732421875</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="0">
+        <v>222.61000061035156</v>
+      </c>
+      <c r="E30" s="0">
+        <v>219.83999633789062</v>
+      </c>
+      <c r="F30" s="0">
+        <v>225.60000610351562</v>
+      </c>
+      <c r="G30" s="0">
+        <v>198.61000061035156</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="0">
+        <v>526.0499877929688</v>
+      </c>
+      <c r="E31" s="0">
+        <v>522.8300170898438</v>
+      </c>
+      <c r="F31" s="0">
+        <v>526.364990234375</v>
+      </c>
+      <c r="G31" s="0">
+        <v>505.4700012207031</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="0">
+        <v>25.780000686645508</v>
+      </c>
+      <c r="E32" s="0">
+        <v>25.6200008392334</v>
+      </c>
+      <c r="F32" s="0">
+        <v>25.850000381469727</v>
+      </c>
+      <c r="G32" s="0">
+        <v>22.357999801635742</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="0">
+        <v>35.47999954223633</v>
+      </c>
+      <c r="E33" s="0">
+        <v>35.36000061035156</v>
+      </c>
+      <c r="F33" s="0">
+        <v>35.93000030517578</v>
+      </c>
+      <c r="G33" s="0">
+        <v>35.369998931884766</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="0">
+        <v>71.94999694824219</v>
+      </c>
+      <c r="E34" s="0">
+        <v>71.23999786376953</v>
+      </c>
+      <c r="F34" s="0">
+        <v>72.72000122070312</v>
+      </c>
+      <c r="G34" s="0">
+        <v>69.19499969482422</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="0">
+        <v>16.290000915527344</v>
+      </c>
+      <c r="E35" s="0">
+        <v>16.110000610351562</v>
+      </c>
+      <c r="F35" s="0">
+        <v>16.5</v>
+      </c>
+      <c r="G35" s="0">
+        <v>15.699999809265137</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="0">
+        <v>318.6300048828125</v>
+      </c>
+      <c r="E36" s="0">
+        <v>317.2200012207031</v>
+      </c>
+      <c r="F36" s="0">
+        <v>318.6700134277344</v>
+      </c>
+      <c r="G36" s="0">
+        <v>311.7200012207031</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="0">
+        <v>67.27999877929688</v>
+      </c>
+      <c r="E37" s="0">
+        <v>66.27999877929688</v>
+      </c>
+      <c r="F37" s="0">
+        <v>67.7249984741211</v>
+      </c>
+      <c r="G37" s="0">
+        <v>62.939998626708984</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="0">
+        <v>106.62999725341797</v>
+      </c>
+      <c r="E38" s="0">
+        <v>106.25</v>
+      </c>
+      <c r="F38" s="0">
+        <v>107.27999877929688</v>
+      </c>
+      <c r="G38" s="0">
+        <v>104.94000244140625</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="0">
+        <v>1176.81005859375</v>
+      </c>
+      <c r="E39" s="0">
+        <v>1162</v>
+      </c>
+      <c r="F39" s="0">
+        <v>1185</v>
+      </c>
+      <c r="G39" s="0">
+        <v>1102.3499755859375</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="0">
+        <v>139.3000030517578</v>
+      </c>
+      <c r="E40" s="0">
+        <v>136.82000732421875</v>
+      </c>
+      <c r="F40" s="0">
+        <v>142.89999389648438</v>
+      </c>
+      <c r="G40" s="0">
+        <v>130.8800048828125</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="0">
+        <v>1.2200000286102295</v>
+      </c>
+      <c r="E41" s="0">
+        <v>1.2100000381469727</v>
+      </c>
+      <c r="F41" s="0">
+        <v>1.2699999809265137</v>
+      </c>
+      <c r="G41" s="0">
+        <v>1.1200000047683716</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="0">
+        <v>224.3000030517578</v>
+      </c>
+      <c r="E42" s="0">
+        <v>223.1999969482422</v>
+      </c>
+      <c r="F42" s="0">
+        <v>225.89999389648438</v>
+      </c>
+      <c r="G42" s="0">
+        <v>212.15499877929688</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="0">
+        <v>45.81999969482422</v>
+      </c>
+      <c r="E43" s="0">
+        <v>44.79999923706055</v>
+      </c>
+      <c r="F43" s="0">
+        <v>47.5</v>
+      </c>
+      <c r="G43" s="0">
+        <v>45.689998626708984</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="0">
+        <v>78.41999816894531</v>
+      </c>
+      <c r="E44" s="0">
+        <v>77.77999877929688</v>
+      </c>
+      <c r="F44" s="0">
+        <v>79.93000030517578</v>
+      </c>
+      <c r="G44" s="0">
+        <v>77.5999984741211</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="0">
+        <v>96.48999786376953</v>
+      </c>
+      <c r="E45" s="0">
+        <v>97.19000244140625</v>
+      </c>
+      <c r="F45" s="0">
+        <v>97.87999725341797</v>
+      </c>
+      <c r="G45" s="0">
+        <v>92.16999816894531</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="0">
+        <v>35.2599983215332</v>
+      </c>
+      <c r="E46" s="0">
+        <v>34.540000915527344</v>
+      </c>
+      <c r="F46" s="0">
+        <v>35.43000030517578</v>
+      </c>
+      <c r="G46" s="0">
+        <v>32.75</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="0">
+        <v>160.05999755859375</v>
+      </c>
+      <c r="E47" s="0">
+        <v>159.86000061035156</v>
+      </c>
+      <c r="F47" s="0">
+        <v>162.27000427246094</v>
+      </c>
+      <c r="G47" s="0">
+        <v>159.6999969482422</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="0">
+        <v>1.8250000476837158</v>
+      </c>
+      <c r="E48" s="0">
+        <v>1.8899999856948853</v>
+      </c>
+      <c r="F48" s="0">
+        <v>2</v>
+      </c>
+      <c r="G48" s="0">
+        <v>1.7999999523162842</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="0">
+        <v>49.68000030517578</v>
+      </c>
+      <c r="E49" s="0">
+        <v>49.400001525878906</v>
+      </c>
+      <c r="F49" s="0">
+        <v>50.369998931884766</v>
+      </c>
+      <c r="G49" s="0">
+        <v>47.970001220703125</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="0">
+        <v>38.36000061035156</v>
+      </c>
+      <c r="E50" s="0">
+        <v>38.2400016784668</v>
+      </c>
+      <c r="F50" s="0">
+        <v>39.02000045776367</v>
+      </c>
+      <c r="G50" s="0">
+        <v>38.11000061035156</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="0">
+        <v>129.3300018310547</v>
+      </c>
+      <c r="E51" s="0">
+        <v>129.92999267578125</v>
+      </c>
+      <c r="F51" s="0">
+        <v>129.92999267578125</v>
+      </c>
+      <c r="G51" s="0">
+        <v>121.66000366210938</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="0">
+        <v>123.79000091552734</v>
+      </c>
+      <c r="E52" s="0">
+        <v>124.0999984741211</v>
+      </c>
+      <c r="F52" s="0">
+        <v>125.91000366210938</v>
+      </c>
+      <c r="G52" s="0">
+        <v>123.37000274658203</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="0">
+        <v>134.42999267578125</v>
+      </c>
+      <c r="E53" s="0">
+        <v>133.94000244140625</v>
+      </c>
+      <c r="F53" s="0">
+        <v>134.42999267578125</v>
+      </c>
+      <c r="G53" s="0">
+        <v>133.0500030517578</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="0">
+        <v>20.3799991607666</v>
+      </c>
+      <c r="E54" s="0">
+        <v>19.860000610351562</v>
+      </c>
+      <c r="F54" s="0">
+        <v>21.18000030517578</v>
+      </c>
+      <c r="G54" s="0">
+        <v>19.530000686645508</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="0">
+        <v>140.1300048828125</v>
+      </c>
+      <c r="E55" s="0">
+        <v>138.5399932861328</v>
+      </c>
+      <c r="F55" s="0">
+        <v>140.1300048828125</v>
+      </c>
+      <c r="G55" s="0">
+        <v>131.22999572753906</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="0">
+        <v>136.13999938964844</v>
+      </c>
+      <c r="E56" s="0">
+        <v>134.49000549316406</v>
+      </c>
+      <c r="F56" s="0">
+        <v>136.64999389648438</v>
+      </c>
+      <c r="G56" s="0">
+        <v>126.31999969482422</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="0">
+        <v>143.38999938964844</v>
+      </c>
+      <c r="E57" s="0">
+        <v>140.8800048828125</v>
+      </c>
+      <c r="F57" s="0">
+        <v>143.85000610351562</v>
+      </c>
+      <c r="G57" s="0">
+        <v>132.8699951171875</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.377994537353516" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.8009033203125" customWidth="1"/>
+    <col min="5" max="5" width="13.641397476196289" customWidth="1"/>
+    <col min="6" max="6" width="11.8009033203125" customWidth="1"/>
+    <col min="7" max="7" width="11.8009033203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0">
+        <v>21.25</v>
+      </c>
+      <c r="E2" s="0">
+        <v>21.809999465942383</v>
+      </c>
+      <c r="F2" s="0">
+        <v>22.915000915527344</v>
+      </c>
+      <c r="G2" s="0">
+        <v>21.020000457763672</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0">
+        <v>8.960000038146973</v>
+      </c>
+      <c r="E3" s="0">
+        <v>9.020000457763672</v>
+      </c>
+      <c r="F3" s="0">
+        <v>11.3149995803833</v>
+      </c>
+      <c r="G3" s="0">
+        <v>8.949999809265137</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0">
+        <v>75.8499984741211</v>
+      </c>
+      <c r="E4" s="0">
+        <v>76.4800033569336</v>
+      </c>
+      <c r="F4" s="0">
+        <v>76.94999694824219</v>
+      </c>
+      <c r="G4" s="0">
+        <v>74.95999908447266</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0">
+        <v>16.780000686645508</v>
+      </c>
+      <c r="E5" s="0">
+        <v>17.450000762939453</v>
+      </c>
+      <c r="F5" s="0">
+        <v>17.969999313354492</v>
+      </c>
+      <c r="G5" s="0">
+        <v>16.559999465942383</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="0">
+        <v>111.36000061035156</v>
+      </c>
+      <c r="E6" s="0">
+        <v>114.77999877929688</v>
+      </c>
+      <c r="F6" s="0">
+        <v>114.87999725341797</v>
+      </c>
+      <c r="G6" s="0">
+        <v>110.38999938964844</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0">
+        <v>138.1699981689453</v>
+      </c>
+      <c r="E7" s="0">
+        <v>142.58999633789062</v>
+      </c>
+      <c r="F7" s="0">
+        <v>142.57989501953125</v>
+      </c>
+      <c r="G7" s="0">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0">
+        <v>90.41000366210938</v>
+      </c>
+      <c r="E8" s="0">
+        <v>90.51000213623047</v>
+      </c>
+      <c r="F8" s="0">
+        <v>91.12999725341797</v>
+      </c>
+      <c r="G8" s="0">
+        <v>89.05999755859375</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0">
+        <v>36.869998931884766</v>
+      </c>
+      <c r="E9" s="0">
+        <v>36.900001525878906</v>
+      </c>
+      <c r="F9" s="0">
+        <v>37.75</v>
+      </c>
+      <c r="G9" s="0">
+        <v>36.630001068115234</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.8700000047683716</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.8700000047683716</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.8700000047683716</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.8100000023841858</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0">
+        <v>128.8699951171875</v>
+      </c>
+      <c r="E11" s="0">
+        <v>130.2100067138672</v>
+      </c>
+      <c r="F11" s="0">
+        <v>131.79629516601562</v>
+      </c>
+      <c r="G11" s="0">
+        <v>127.23999786376953</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0">
+        <v>36.90999984741211</v>
+      </c>
+      <c r="E12" s="0">
+        <v>37.02000045776367</v>
+      </c>
+      <c r="F12" s="0">
+        <v>38.220001220703125</v>
+      </c>
+      <c r="G12" s="0">
+        <v>36.90999984741211</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0">
+        <v>44.790000915527344</v>
+      </c>
+      <c r="E13" s="0">
+        <v>45.61000061035156</v>
+      </c>
+      <c r="F13" s="0">
+        <v>47.21500015258789</v>
+      </c>
+      <c r="G13" s="0">
+        <v>44.52000045776367</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0">
+        <v>193.88999938964844</v>
+      </c>
+      <c r="E14" s="0">
+        <v>198.4600067138672</v>
+      </c>
+      <c r="F14" s="0">
+        <v>202.8000030517578</v>
+      </c>
+      <c r="G14" s="0">
+        <v>192.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="0">
+        <v>193.3300018310547</v>
+      </c>
+      <c r="E15" s="0">
+        <v>199.17999267578125</v>
+      </c>
+      <c r="F15" s="0">
+        <v>201.09500122070312</v>
+      </c>
+      <c r="G15" s="0">
+        <v>190.5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="0">
+        <v>280.9800109863281</v>
+      </c>
+      <c r="E16" s="0">
+        <v>282.1400146484375</v>
+      </c>
+      <c r="F16" s="0">
+        <v>288.05999755859375</v>
+      </c>
+      <c r="G16" s="0">
+        <v>277.75</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0">
+        <v>266.20001220703125</v>
+      </c>
+      <c r="E17" s="0">
+        <v>268.2900085449219</v>
+      </c>
+      <c r="F17" s="0">
+        <v>275.0199890136719</v>
+      </c>
+      <c r="G17" s="0">
+        <v>263.94000244140625</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="0">
+        <v>194.75</v>
+      </c>
+      <c r="E18" s="0">
+        <v>202.8800048828125</v>
+      </c>
+      <c r="F18" s="0">
+        <v>205.81500244140625</v>
+      </c>
+      <c r="G18" s="0">
+        <v>190.5399932861328</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="0">
+        <v>58.47999954223633</v>
+      </c>
+      <c r="E19" s="0">
+        <v>58.619998931884766</v>
+      </c>
+      <c r="F19" s="0">
+        <v>60.27000045776367</v>
+      </c>
+      <c r="G19" s="0">
+        <v>58.150001525878906</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="0">
+        <v>123.48999786376953</v>
+      </c>
+      <c r="E20" s="0">
+        <v>120.33999633789062</v>
+      </c>
+      <c r="F20" s="0">
+        <v>187.5</v>
+      </c>
+      <c r="G20" s="0">
+        <v>116.9000015258789</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="0">
+        <v>2029.050048828125</v>
+      </c>
+      <c r="E21" s="0">
+        <v>2032.530029296875</v>
+      </c>
+      <c r="F21" s="0">
+        <v>2045.6400146484375</v>
+      </c>
+      <c r="G21" s="0">
+        <v>1996.0899658203125</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="0">
+        <v>80.11000061035156</v>
+      </c>
+      <c r="E22" s="0">
+        <v>80.45999908447266</v>
+      </c>
+      <c r="F22" s="0">
+        <v>82.69499969482422</v>
+      </c>
+      <c r="G22" s="0">
+        <v>78.18000030517578</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0">
+        <v>293.0299987792969</v>
+      </c>
+      <c r="E23" s="0">
+        <v>292.75</v>
+      </c>
+      <c r="F23" s="0">
+        <v>297.8786926269531</v>
+      </c>
+      <c r="G23" s="0">
+        <v>292.4549865722656</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="0">
+        <v>51.70000076293945</v>
+      </c>
+      <c r="E24" s="0">
+        <v>51.52000045776367</v>
+      </c>
+      <c r="F24" s="0">
+        <v>52.060001373291016</v>
+      </c>
+      <c r="G24" s="0">
+        <v>51.16999816894531</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="0">
+        <v>86.48999786376953</v>
+      </c>
+      <c r="E25" s="0">
+        <v>89.27999877929688</v>
+      </c>
+      <c r="F25" s="0">
+        <v>92.29900360107422</v>
+      </c>
+      <c r="G25" s="0">
+        <v>84.69999694824219</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="0">
+        <v>56.61000061035156</v>
+      </c>
+      <c r="E26" s="0">
+        <v>57.70000076293945</v>
+      </c>
+      <c r="F26" s="0">
+        <v>59.959999084472656</v>
+      </c>
+      <c r="G26" s="0">
+        <v>56.41999816894531</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="0">
+        <v>225.14999389648438</v>
+      </c>
+      <c r="E27" s="0">
+        <v>224.0500030517578</v>
+      </c>
+      <c r="F27" s="0">
+        <v>225.32000732421875</v>
+      </c>
+      <c r="G27" s="0">
+        <v>222.44000244140625</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="0">
+        <v>127.33000183105469</v>
+      </c>
+      <c r="E28" s="0">
+        <v>131.61000061035156</v>
+      </c>
+      <c r="F28" s="0">
+        <v>134.30999755859375</v>
+      </c>
+      <c r="G28" s="0">
+        <v>126.41999816894531</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="0">
+        <v>235.3000030517578</v>
+      </c>
+      <c r="E29" s="0">
+        <v>235.4600067138672</v>
+      </c>
+      <c r="F29" s="0">
+        <v>236.94000244140625</v>
+      </c>
+      <c r="G29" s="0">
+        <v>231.57000732421875</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="0">
+        <v>188.25</v>
+      </c>
+      <c r="E30" s="0">
+        <v>200.24000549316406</v>
+      </c>
+      <c r="F30" s="0">
+        <v>202.49989318847656</v>
+      </c>
+      <c r="G30" s="0">
+        <v>159.08999633789062</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="0">
+        <v>499.9800109863281</v>
+      </c>
+      <c r="E31" s="0">
+        <v>505.7200012207031</v>
+      </c>
+      <c r="F31" s="0">
+        <v>508.5899963378906</v>
+      </c>
+      <c r="G31" s="0">
+        <v>490.8800048828125</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="0">
+        <v>21.3700008392334</v>
+      </c>
+      <c r="E32" s="0">
+        <v>22.510000228881836</v>
+      </c>
+      <c r="F32" s="0">
+        <v>23.219999313354492</v>
+      </c>
+      <c r="G32" s="0">
+        <v>20.600000381469727</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="0">
+        <v>35.650001525878906</v>
+      </c>
+      <c r="E33" s="0">
+        <v>35.61000061035156</v>
+      </c>
+      <c r="F33" s="0">
+        <v>35.790000915527344</v>
+      </c>
+      <c r="G33" s="0">
+        <v>35.25</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="0">
+        <v>66.375</v>
+      </c>
+      <c r="E34" s="0">
+        <v>69.5999984741211</v>
+      </c>
+      <c r="F34" s="0">
+        <v>68.91000366210938</v>
+      </c>
+      <c r="G34" s="0">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="0">
+        <v>15.260000228881836</v>
+      </c>
+      <c r="E35" s="0">
+        <v>15.699999809265137</v>
+      </c>
+      <c r="F35" s="0">
+        <v>16.100000381469727</v>
+      </c>
+      <c r="G35" s="0">
+        <v>15.220999717712402</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="0">
+        <v>309.9679870605469</v>
+      </c>
+      <c r="E36" s="0">
+        <v>311.8699951171875</v>
+      </c>
+      <c r="F36" s="0">
+        <v>312.885009765625</v>
+      </c>
+      <c r="G36" s="0">
+        <v>307.389892578125</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="0">
+        <v>61.02000045776367</v>
+      </c>
+      <c r="E37" s="0">
+        <v>63.15999984741211</v>
+      </c>
+      <c r="F37" s="0">
+        <v>64.93090057373047</v>
+      </c>
+      <c r="G37" s="0">
+        <v>59.470001220703125</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="0">
+        <v>105.00700378417969</v>
+      </c>
+      <c r="E38" s="0">
+        <v>104.97000122070312</v>
+      </c>
+      <c r="F38" s="0">
+        <v>107.69999694824219</v>
+      </c>
+      <c r="G38" s="0">
+        <v>104.05999755859375</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="0">
+        <v>1090.0799560546875</v>
+      </c>
+      <c r="E39" s="0">
+        <v>1106.010009765625</v>
+      </c>
+      <c r="F39" s="0">
+        <v>1103.989990234375</v>
+      </c>
+      <c r="G39" s="0">
+        <v>1051.2501220703125</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="0">
+        <v>127.41999816894531</v>
+      </c>
+      <c r="E40" s="0">
+        <v>131.30999755859375</v>
+      </c>
+      <c r="F40" s="0">
+        <v>138.64999389648438</v>
+      </c>
+      <c r="G40" s="0">
+        <v>125.12999725341797</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="0">
+        <v>1.0700000524520874</v>
+      </c>
+      <c r="E41" s="0">
+        <v>1.125</v>
+      </c>
+      <c r="F41" s="0">
+        <v>1.2200000286102295</v>
+      </c>
+      <c r="G41" s="0">
+        <v>1.059999942779541</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="0">
+        <v>204.60000610351562</v>
+      </c>
+      <c r="E42" s="0">
+        <v>213.50999450683594</v>
+      </c>
+      <c r="F42" s="0">
+        <v>211.9600067138672</v>
+      </c>
+      <c r="G42" s="0">
+        <v>202.10000610351562</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="0">
+        <v>45.810001373291016</v>
+      </c>
+      <c r="E43" s="0">
+        <v>46.06999969482422</v>
+      </c>
+      <c r="F43" s="0">
+        <v>47.900001525878906</v>
+      </c>
+      <c r="G43" s="0">
+        <v>45.25</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="0">
+        <v>76.91000366210938</v>
+      </c>
+      <c r="E44" s="0">
+        <v>77.6500015258789</v>
+      </c>
+      <c r="F44" s="0">
+        <v>79.86000061035156</v>
+      </c>
+      <c r="G44" s="0">
+        <v>76.69000244140625</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="0">
+        <v>90</v>
+      </c>
+      <c r="E45" s="0">
+        <v>92.70999908447266</v>
+      </c>
+      <c r="F45" s="0">
+        <v>92.05999755859375</v>
+      </c>
+      <c r="G45" s="0">
+        <v>88.28679656982422</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="0">
+        <v>32.630001068115234</v>
+      </c>
+      <c r="E46" s="0">
+        <v>33</v>
+      </c>
+      <c r="F46" s="0">
+        <v>34.20000076293945</v>
+      </c>
+      <c r="G46" s="0">
+        <v>32.02000045776367</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="0">
+        <v>159.5</v>
+      </c>
+      <c r="E47" s="0">
+        <v>159.91000366210938</v>
+      </c>
+      <c r="F47" s="0">
+        <v>163.64999389648438</v>
+      </c>
+      <c r="G47" s="0">
+        <v>158.6999969482422</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="0">
+        <v>2</v>
+      </c>
+      <c r="E48" s="0">
+        <v>1.9871000051498413</v>
+      </c>
+      <c r="F48" s="0">
+        <v>2.0199999809265137</v>
+      </c>
+      <c r="G48" s="0">
+        <v>1.909999966621399</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" s="0">
+        <v>47.400001525878906</v>
+      </c>
+      <c r="E49" s="0">
+        <v>48.09000015258789</v>
+      </c>
+      <c r="F49" s="0">
+        <v>49.90999984741211</v>
+      </c>
+      <c r="G49" s="0">
+        <v>47.29999923706055</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="0">
+        <v>37.970001220703125</v>
+      </c>
+      <c r="E50" s="0">
+        <v>38.119998931884766</v>
+      </c>
+      <c r="F50" s="0">
+        <v>39.36000061035156</v>
+      </c>
+      <c r="G50" s="0">
+        <v>37.779998779296875</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="0">
+        <v>124.41000366210938</v>
+      </c>
+      <c r="E51" s="0">
+        <v>125.8499984741211</v>
+      </c>
+      <c r="F51" s="0">
+        <v>124.41000366210938</v>
+      </c>
+      <c r="G51" s="0">
+        <v>120.48149871826172</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="0">
+        <v>125.43000030517578</v>
+      </c>
+      <c r="E52" s="0">
+        <v>124.81999969482422</v>
+      </c>
+      <c r="F52" s="0">
+        <v>127.55999755859375</v>
+      </c>
+      <c r="G52" s="0">
+        <v>124.42500305175781</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="0">
+        <v>133.25999450683594</v>
+      </c>
+      <c r="E53" s="0">
+        <v>133.11000061035156</v>
+      </c>
+      <c r="F53" s="0">
+        <v>134.5301055908203</v>
+      </c>
+      <c r="G53" s="0">
+        <v>132.8699951171875</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="0">
+        <v>19.18000030517578</v>
+      </c>
+      <c r="E54" s="0">
+        <v>19.56999969482422</v>
+      </c>
+      <c r="F54" s="0">
+        <v>20.66990089416504</v>
+      </c>
+      <c r="G54" s="0">
+        <v>18.610000610351562</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="0">
+        <v>129.57000732421875</v>
+      </c>
+      <c r="E55" s="0">
+        <v>131.4199981689453</v>
+      </c>
+      <c r="F55" s="0">
+        <v>135.39999389648438</v>
+      </c>
+      <c r="G55" s="0">
+        <v>128.6750030517578</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="0">
+        <v>122.7300033569336</v>
+      </c>
+      <c r="E56" s="0">
+        <v>127.36000061035156</v>
+      </c>
+      <c r="F56" s="0">
+        <v>127.57990264892578</v>
+      </c>
+      <c r="G56" s="0">
+        <v>120.22000122070312</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D57" s="0">
+        <v>129.3699951171875</v>
+      </c>
+      <c r="E57" s="0">
+        <v>133.22000122070312</v>
+      </c>
+      <c r="F57" s="0">
+        <v>134.22000122070312</v>
+      </c>
+      <c r="G57" s="0">
+        <v>126.61000061035156</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:G57"/>

</xml_diff>